<commit_message>
Use UniProt REST services to improve speed of mapping fetching.
Former-commit-id: 52112c9e4f10334bb3d8f5ad34c10e2acbfdf65f
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data_uniprot.xlsx
+++ b/src/test/resources/data/data_uniprot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="21320" windowHeight="8260"/>
@@ -30,7 +30,7 @@
     <t>sp|P11171</t>
   </si>
   <si>
-    <t>sp|Q08211</t>
+    <t>tr|Q08211</t>
   </si>
 </sst>
 </file>

</xml_diff>